<commit_message>
Second Maintenance update of vkyc,vpd and Reschedule cases
</commit_message>
<xml_diff>
--- a/documents/importing_sample_data_front_end(HFCL).xlsx
+++ b/documents/importing_sample_data_front_end(HFCL).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
   <si>
     <t xml:space="preserve">case_name</t>
   </si>
@@ -62,6 +62,12 @@
   </si>
   <si>
     <t xml:space="preserve">guarantor_coapplicant_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">business_manager_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">business_manager_mobile_no</t>
   </si>
   <si>
     <t xml:space="preserve">admin_comment</t>
@@ -284,30 +290,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:O65536"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.9795918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.7397959183673"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.6530612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.5510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="27.2704081632653"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.8214285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="20.5204081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="19.7091836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.4642857142857"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="20.3826530612245"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="17.280612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="26.8622448979592"/>
+    <col collapsed="false" hidden="false" max="17" min="15" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="20.25"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -353,13 +359,19 @@
       <c r="N1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>14</v>
       </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>6</v>
@@ -371,51 +383,45 @@
         <v>1</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>9631261010</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="K2" s="0" t="n">
         <v>111</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="N2" s="0" t="n">
         <v>111</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
+      </c>
+      <c r="P2" s="0" t="n">
+        <v>9835677898</v>
+      </c>
+      <c r="Q2" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="shashi.ranjan@mailinator.com"/>

</xml_diff>